<commit_message>
adding my picture and name in to the team section
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -127,12 +127,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -140,14 +140,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -336,7 +336,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -353,7 +353,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -371,7 +371,7 @@
       <font>
         <b/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,7 +515,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -550,7 +549,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -726,22 +724,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="21">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -752,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -761,7 +759,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="30">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -772,7 +770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="45">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -781,7 +779,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="45">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -790,7 +788,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="45">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -799,7 +797,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -810,7 +808,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -821,7 +819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="45">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -830,7 +828,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -839,7 +837,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="45">
       <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
@@ -848,7 +846,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
@@ -857,7 +855,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
@@ -866,7 +864,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
@@ -877,7 +875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="45">
       <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
@@ -886,7 +884,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
@@ -897,16 +895,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
@@ -924,7 +924,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="10" t="s">
         <v>33</v>
       </c>
@@ -935,7 +935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -944,17 +944,17 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="10"/>
       <c r="B22" s="12"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="10"/>
       <c r="B23" s="12"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="9"/>

</xml_diff>

<commit_message>
change the Photo & Name
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -127,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,7 +336,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -353,7 +353,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -371,7 +371,7 @@
       <font>
         <b/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -483,7 +483,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,9 +515,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,6 +550,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -724,14 +726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="3" customWidth="1"/>
@@ -739,7 +741,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -750,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -759,7 +761,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -770,7 +772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -779,7 +781,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" ht="45">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -788,7 +790,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -797,7 +799,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -808,7 +810,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -819,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -828,7 +830,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -837,7 +839,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="45">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
@@ -846,7 +848,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
@@ -855,7 +857,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
@@ -864,7 +866,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
@@ -875,7 +877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
@@ -884,7 +886,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
@@ -895,7 +897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
@@ -906,16 +908,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
@@ -924,7 +928,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>33</v>
       </c>
@@ -935,7 +939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -944,17 +948,17 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="12"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="12"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="9"/>

</xml_diff>